<commit_message>
Pequenas coisas que nao foram nos commits anteriores, por algum motivo.
</commit_message>
<xml_diff>
--- a/Docs Auxiliares/queries_modulos_andre.xlsx
+++ b/Docs Auxiliares/queries_modulos_andre.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="15345" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -232,8 +232,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -910,6 +922,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -918,12 +963,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -985,28 +1024,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1018,16 +1036,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1036,6 +1054,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1313,7 +1336,7 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -1332,38 +1355,38 @@
   <sheetData>
     <row r="1" spans="1:16384" ht="39.75" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54" t="s">
+      <c r="K1" s="61"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="56"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="65"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -17736,14 +17759,14 @@
     </row>
     <row r="2" spans="1:16384" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="50"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
@@ -17753,9 +17776,9 @@
       <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="59"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="68"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -34127,84 +34150,84 @@
       <c r="XFD2" s="3"/>
     </row>
     <row r="3" spans="1:16384" ht="20.100000000000001" customHeight="1" thickTop="1">
-      <c r="A3" s="40"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="68"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="62"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="7"/>
       <c r="J3" s="8"/>
       <c r="K3" s="9"/>
       <c r="L3" s="10"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="44"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="53"/>
     </row>
     <row r="4" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="41"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="70"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="14"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="64"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="37"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
       <c r="P4" s="20">
         <f t="shared" ref="P4:P14" si="0">K4*1000</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="73" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="44" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
-      <c r="G5" s="65"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="26"/>
       <c r="I5" s="27"/>
       <c r="J5" s="17"/>
       <c r="K5" s="18"/>
       <c r="L5" s="19"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="37"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="48"/>
       <c r="P5" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="38"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="43" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="23" t="s">
@@ -34213,21 +34236,21 @@
       <c r="E6" s="24"/>
       <c r="F6" s="25"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="66"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="27"/>
       <c r="J6" s="17"/>
       <c r="K6" s="18"/>
       <c r="L6" s="19"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="37"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="48"/>
       <c r="P6" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="38"/>
+      <c r="A7" s="73"/>
       <c r="B7" s="21" t="s">
         <v>22</v>
       </c>
@@ -34240,75 +34263,75 @@
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="64"/>
+      <c r="H7" s="39"/>
       <c r="I7" s="16"/>
       <c r="J7" s="17"/>
       <c r="K7" s="18"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="37"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="48"/>
       <c r="P7" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="38"/>
+      <c r="A8" s="73"/>
       <c r="B8" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="45" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="66"/>
+      <c r="H8" s="41"/>
       <c r="I8" s="16"/>
       <c r="J8" s="17"/>
       <c r="K8" s="18"/>
       <c r="L8" s="19"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="37"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="48"/>
       <c r="P8" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="38"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="44" t="s">
         <v>43</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
       <c r="I9" s="27"/>
       <c r="J9" s="17"/>
       <c r="K9" s="18"/>
       <c r="L9" s="19"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="37"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="48"/>
       <c r="P9" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="38"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="21" t="s">
         <v>29</v>
       </c>
@@ -34320,22 +34343,22 @@
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="66"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="76"/>
       <c r="I10" s="27"/>
       <c r="J10" s="17"/>
       <c r="K10" s="18"/>
       <c r="L10" s="19"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="36"/>
-      <c r="O10" s="37"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="48"/>
       <c r="P10" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="38"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="21" t="s">
         <v>32</v>
       </c>
@@ -34348,21 +34371,21 @@
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="64"/>
+      <c r="H11" s="39"/>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="37"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="48"/>
       <c r="P11" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="38"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="21" t="s">
         <v>35</v>
       </c>
@@ -34374,22 +34397,22 @@
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="64"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
       <c r="I12" s="16"/>
       <c r="J12" s="17"/>
       <c r="K12" s="18"/>
       <c r="L12" s="19"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="37"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="48"/>
       <c r="P12" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="38"/>
+      <c r="A13" s="73"/>
       <c r="B13" s="21" t="s">
         <v>37</v>
       </c>
@@ -34402,21 +34425,21 @@
       <c r="E13" s="24"/>
       <c r="F13" s="25"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="64"/>
+      <c r="H13" s="39"/>
       <c r="I13" s="27"/>
       <c r="J13" s="17"/>
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="37"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="48"/>
       <c r="P13" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:16384" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="39"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="28" t="s">
         <v>39</v>
       </c>
@@ -34429,14 +34452,14 @@
       <c r="E14" s="31"/>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
-      <c r="H14" s="67"/>
+      <c r="H14" s="42"/>
       <c r="I14" s="33"/>
       <c r="J14" s="17"/>
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="37"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="48"/>
       <c r="P14" s="20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -67217,6 +67240,17 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="25">
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M10:O10"/>
     <mergeCell ref="M4:O4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="M3:O3"/>
@@ -67231,17 +67265,6 @@
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M1:O2"/>
     <mergeCell ref="C3:D4"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M10:O10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" cellComments="asDisplayed" r:id="rId1"/>

</xml_diff>